<commit_message>
added analysis and joining
</commit_message>
<xml_diff>
--- a/index_data_2015.xlsx
+++ b/index_data_2015.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnab\Desktop\Data Science\Practice\Board Diversity Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B456DF1-921B-4B0F-A9A9-9E73C41F9F01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87827FF-8532-49A7-9128-833C0BF9C04B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26460" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="5" r:id="rId1"/>
@@ -22,33 +22,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
-    <t>ICICI BANK LTD.</t>
-  </si>
-  <si>
     <t>INDUSIND BANK LTD.</t>
   </si>
   <si>
-    <t>KARNATAKA BANK LTD.,THE</t>
-  </si>
-  <si>
-    <t>KARUR VYSYA BANK LTD.,THE</t>
-  </si>
-  <si>
     <t>AXIS BANK LTD.</t>
   </si>
   <si>
     <t>YES BANK LTD.</t>
   </si>
   <si>
-    <t>DCB BANK LTD.</t>
-  </si>
-  <si>
-    <t>IDBI BANK LTD.</t>
-  </si>
-  <si>
-    <t>LAKSHMI VILAS BANK LTD.,THE</t>
-  </si>
-  <si>
     <t>BANK OF BARODA</t>
   </si>
   <si>
@@ -58,9 +40,6 @@
     <t>CANARA BANK</t>
   </si>
   <si>
-    <t>FEDERAL BANK LTD.,THE</t>
-  </si>
-  <si>
     <t>STATE BANK OF INDIA</t>
   </si>
   <si>
@@ -70,15 +49,9 @@
     <t>BANK OF INDIA</t>
   </si>
   <si>
-    <t>SOUTH INDIAN BANK LTD.,THE</t>
-  </si>
-  <si>
     <t>CORPORATION BANK</t>
   </si>
   <si>
-    <t>HDFC BANK LTD.</t>
-  </si>
-  <si>
     <t>INDIAN OVERSEAS BANK</t>
   </si>
   <si>
@@ -109,9 +82,6 @@
     <t>SYNDICATE BANK</t>
   </si>
   <si>
-    <t>JAMMU &amp; KASHMIR BANK LTD.,THE</t>
-  </si>
-  <si>
     <t>DHANLAXMI BANK LTD.</t>
   </si>
   <si>
@@ -185,6 +155,36 @@
   </si>
   <si>
     <t>Quartiles</t>
+  </si>
+  <si>
+    <t>KARUR VYSYA BANK LTD.</t>
+  </si>
+  <si>
+    <t>I C I C I BANK LTD.</t>
+  </si>
+  <si>
+    <t>LAKSHMI VILAS BANK LTD.</t>
+  </si>
+  <si>
+    <t>D C B BANK LTD.</t>
+  </si>
+  <si>
+    <t>H D F C BANK LTD.</t>
+  </si>
+  <si>
+    <t>I D B I BANK LTD.</t>
+  </si>
+  <si>
+    <t>FEDERAL BANK LTD.</t>
+  </si>
+  <si>
+    <t>KARNATAKA BANK LTD.</t>
+  </si>
+  <si>
+    <t>SOUTH INDIAN BANK LTD.</t>
+  </si>
+  <si>
+    <t>JAMMU &amp; KASHMIR BANK LTD.</t>
   </si>
 </sst>
 </file>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,39 +621,39 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C2" s="6">
         <v>0.97061220000000004</v>
@@ -674,15 +674,15 @@
         <v>-2.2655959999999999</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C3" s="6">
         <v>0.99773239999999996</v>
@@ -704,7 +704,7 @@
       </c>
       <c r="I3" s="8"/>
       <c r="K3" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="L3" s="2">
         <f>QUARTILE(H2:H41,1)</f>
@@ -713,10 +713,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6">
         <v>0.98070990000000002</v>
@@ -738,7 +738,7 @@
       </c>
       <c r="I4" s="8"/>
       <c r="K4" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="L4" s="2">
         <f>QUARTILE(H2:H41,2)</f>
@@ -747,10 +747,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C5" s="6">
         <v>0.99691359999999996</v>
@@ -772,7 +772,7 @@
       </c>
       <c r="I5" s="8"/>
       <c r="K5" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="L5" s="2">
         <f>QUARTILE(H2:H41,3)</f>
@@ -781,10 +781,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C6" s="6">
         <v>0.99793390000000004</v>
@@ -806,7 +806,7 @@
       </c>
       <c r="I6" s="8"/>
       <c r="K6" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="L6" s="2">
         <f>QUARTILE(H2:H41,4)</f>
@@ -815,10 +815,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C7" s="6">
         <v>0.99691359999999996</v>
@@ -842,10 +842,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C8" s="6">
         <v>0.99243859999999995</v>
@@ -869,10 +869,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C9" s="6">
         <v>0.99408289999999999</v>
@@ -896,10 +896,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C10" s="6">
         <v>0.98530759999999995</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6">
         <v>0.99653979999999998</v>
@@ -950,10 +950,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C12" s="6">
         <v>0.99</v>
@@ -974,15 +974,15 @@
         <v>-0.4023948</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C13" s="6">
         <v>0.99</v>
@@ -1006,10 +1006,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C14" s="6">
         <v>0.99092970000000002</v>
@@ -1033,10 +1033,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C15" s="6">
         <v>0.98765429999999999</v>
@@ -1060,10 +1060,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C16" s="6">
         <v>0.99793390000000004</v>
@@ -1087,10 +1087,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C17" s="6">
         <v>0.99555559999999998</v>
@@ -1114,10 +1114,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C18" s="6">
         <v>0.99437500000000001</v>
@@ -1141,10 +1141,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C19" s="6">
         <v>0.99673469999999997</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C20" s="6">
         <v>0.99713010000000002</v>
@@ -1195,10 +1195,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C21" s="6">
         <v>0.99360000000000004</v>
@@ -1222,10 +1222,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C22" s="6">
         <v>0.99625160000000001</v>
@@ -1246,15 +1246,15 @@
         <v>0.21010390000000001</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C23" s="6">
         <v>0.99464609999999998</v>
@@ -1278,10 +1278,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C24" s="6">
         <v>0.99639999999999995</v>
@@ -1305,10 +1305,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C25" s="6">
         <v>0.99653979999999998</v>
@@ -1332,10 +1332,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C26" s="6">
         <v>0.99667159999999999</v>
@@ -1359,10 +1359,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C27" s="6">
         <v>0.99653979999999998</v>
@@ -1386,10 +1386,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C28" s="6">
         <v>0.99535130000000005</v>
@@ -1413,10 +1413,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C29" s="6">
         <v>0.99653979999999998</v>
@@ -1440,10 +1440,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C30" s="6">
         <v>0.99134670000000003</v>
@@ -1467,10 +1467,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C31" s="6">
         <v>0.99592579999999997</v>
@@ -1494,10 +1494,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C32" s="6">
         <v>0.99134670000000003</v>
@@ -1518,15 +1518,15 @@
         <v>0.83797710000000003</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C33" s="6">
         <v>0.99464609999999998</v>
@@ -1550,10 +1550,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C34" s="6">
         <v>0.99793390000000004</v>
@@ -1577,10 +1577,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C35" s="6">
         <v>0.99555559999999998</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C36" s="6">
         <v>0.99555559999999998</v>
@@ -1631,10 +1631,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C37" s="6">
         <v>0.99857600000000002</v>
@@ -1658,10 +1658,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C38" s="6">
         <v>0.99437500000000001</v>
@@ -1685,10 +1685,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C39" s="6">
         <v>0.99773239999999996</v>
@@ -1712,10 +1712,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C40" s="6">
         <v>0.99773239999999996</v>
@@ -1739,10 +1739,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C41" s="6">
         <v>1</v>

</xml_diff>